<commit_message>
fix tests, added stable hash for names
</commit_message>
<xml_diff>
--- a/examples/protocols/multicolor-particle-calibration/artifacts/multicolor-particle-calibration_template.xlsx
+++ b/examples/protocols/multicolor-particle-calibration/artifacts/multicolor-particle-calibration_template.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.138</t>
+          <t>MeasureFluorescence.measurements.862</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.586</t>
+          <t>MeasureFluorescence.measurements.18</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.404</t>
+          <t>MeasureFluorescence.measurements.824</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -8859,7 +8859,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureAbsorbance.measurements.128</t>
+          <t>MeasureAbsorbance.measurements.341</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -11805,7 +11805,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.138</t>
+          <t>MeasureFluorescence.measurements.862</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -11855,17 +11855,17 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.586</t>
+          <t>MeasureFluorescence.measurements.18</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.404</t>
+          <t>MeasureFluorescence.measurements.824</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>MeasureAbsorbance.measurements.128</t>
+          <t>MeasureAbsorbance.measurements.341</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -16605,7 +16605,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.138</t>
+          <t>MeasureFluorescence.measurements.862</t>
         </is>
       </c>
     </row>
@@ -16804,7 +16804,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.586</t>
+          <t>MeasureFluorescence.measurements.18</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -17378,7 +17378,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.586</t>
+          <t>MeasureFluorescence.measurements.18</t>
         </is>
       </c>
     </row>
@@ -17577,7 +17577,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.404</t>
+          <t>MeasureFluorescence.measurements.824</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -18151,7 +18151,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.404</t>
+          <t>MeasureFluorescence.measurements.824</t>
         </is>
       </c>
     </row>
@@ -18350,7 +18350,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureAbsorbance.measurements.128</t>
+          <t>MeasureAbsorbance.measurements.341</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -18674,7 +18674,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureAbsorbance.measurements.128</t>
+          <t>MeasureAbsorbance.measurements.341</t>
         </is>
       </c>
     </row>
@@ -18873,7 +18873,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>MeasureFluorescence.measurements.138</t>
+          <t>MeasureFluorescence.measurements.862</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">

</xml_diff>